<commit_message>
Import some images into resource library
See "元素对应情况"
</commit_message>
<xml_diff>
--- a/EldersAmbition/map/元素对应情况.xlsx
+++ b/EldersAmbition/map/元素对应情况.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="148">
   <si>
     <t>VB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -587,6 +587,14 @@
   </si>
   <si>
     <t>an.f5</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像是否已导入资源库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -665,7 +673,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -707,7 +715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,7 +750,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,23 +959,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -977,136 +991,187 @@
       <c r="C2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1179,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1130,7 +1195,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1138,7 +1203,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1146,7 +1211,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1154,7 +1219,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1227,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1170,7 +1235,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1178,7 +1243,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1186,7 +1251,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1197,7 +1262,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1205,7 +1270,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1213,7 +1278,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1221,7 +1286,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1231,32 +1296,44 @@
       <c r="C35" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>65</v>
       </c>
       <c r="B36" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>66</v>
       </c>
       <c r="B37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>67</v>
       </c>
       <c r="B38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1264,7 +1341,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1275,7 +1352,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1286,7 +1363,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1294,7 +1371,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -1302,7 +1379,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -1310,7 +1387,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1318,7 +1395,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Import all other images into resource library, fix some errors
</commit_message>
<xml_diff>
--- a/EldersAmbition/map/元素对应情况.xlsx
+++ b/EldersAmbition/map/元素对应情况.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="154">
   <si>
     <t>VB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -586,14 +586,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像是否已导入资源库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隔壁学生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺一个？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿色的密码锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时就用完全版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换成叉烧包OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>an.f5</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图像是否已导入资源库</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -959,15 +984,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E40"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -978,7 +1004,7 @@
         <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -992,7 +1018,7 @@
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1003,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1014,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1025,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1036,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1047,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1058,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1069,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1080,7 +1106,7 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1091,7 +1117,7 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1102,7 +1128,7 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1113,7 +1139,7 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1124,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1135,7 +1161,7 @@
         <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1146,7 +1172,7 @@
         <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1157,7 +1183,7 @@
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1168,7 +1194,7 @@
         <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1178,6 +1204,12 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
@@ -1186,6 +1218,12 @@
       <c r="B20" t="s">
         <v>37</v>
       </c>
+      <c r="D20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
@@ -1194,6 +1232,12 @@
       <c r="B21" t="s">
         <v>39</v>
       </c>
+      <c r="D21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -1202,6 +1246,12 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
@@ -1210,6 +1260,12 @@
       <c r="B23" t="s">
         <v>43</v>
       </c>
+      <c r="D23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
@@ -1218,6 +1274,12 @@
       <c r="B24" t="s">
         <v>45</v>
       </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
@@ -1226,6 +1288,12 @@
       <c r="B25" t="s">
         <v>47</v>
       </c>
+      <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
@@ -1234,6 +1302,12 @@
       <c r="B26" t="s">
         <v>49</v>
       </c>
+      <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
@@ -1242,6 +1316,12 @@
       <c r="B27" t="s">
         <v>51</v>
       </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
@@ -1250,6 +1330,9 @@
       <c r="B28" t="s">
         <v>53</v>
       </c>
+      <c r="E28" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
@@ -1261,6 +1344,9 @@
       <c r="C30" t="s">
         <v>101</v>
       </c>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
@@ -1269,6 +1355,9 @@
       <c r="B31" t="s">
         <v>59</v>
       </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
@@ -1277,6 +1366,9 @@
       <c r="B32" t="s">
         <v>61</v>
       </c>
+      <c r="E32" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
@@ -1285,6 +1377,9 @@
       <c r="B33" t="s">
         <v>63</v>
       </c>
+      <c r="E33" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
@@ -1297,7 +1392,7 @@
         <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -1308,7 +1403,7 @@
         <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -1319,7 +1414,7 @@
         <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -1330,7 +1425,7 @@
         <v>97</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1340,6 +1435,12 @@
       <c r="B39" t="s">
         <v>94</v>
       </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
@@ -1351,6 +1452,9 @@
       <c r="C41" t="s">
         <v>99</v>
       </c>
+      <c r="E41" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
@@ -1362,6 +1466,9 @@
       <c r="C42" t="s">
         <v>103</v>
       </c>
+      <c r="E42" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
@@ -1370,6 +1477,9 @@
       <c r="B44" t="s">
         <v>132</v>
       </c>
+      <c r="E44" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
@@ -1378,6 +1488,9 @@
       <c r="B45" t="s">
         <v>134</v>
       </c>
+      <c r="E45" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
@@ -1386,6 +1499,9 @@
       <c r="B46" t="s">
         <v>130</v>
       </c>
+      <c r="E46" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
@@ -1394,6 +1510,9 @@
       <c r="B47" t="s">
         <v>133</v>
       </c>
+      <c r="E47" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
@@ -1402,32 +1521,44 @@
       <c r="B48" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>79</v>
       </c>
       <c r="B49" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>80</v>
       </c>
       <c r="B50" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>81</v>
       </c>
       <c r="B51" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -1437,8 +1568,11 @@
       <c r="D52" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E52" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -1448,24 +1582,33 @@
       <c r="C54" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>72</v>
       </c>
       <c r="B55" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>73</v>
       </c>
       <c r="B56" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>91</v>
       </c>
@@ -1475,8 +1618,11 @@
       <c r="D58" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>92</v>
       </c>
@@ -1486,41 +1632,56 @@
       <c r="C59" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E59" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>89</v>
       </c>
       <c r="B61" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E61" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>90</v>
       </c>
       <c r="B62" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E62" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>122</v>
       </c>
       <c r="B63" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E63" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>124</v>
       </c>
       <c r="B64" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -1530,59 +1691,86 @@
       <c r="C66" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E66" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>86</v>
       </c>
       <c r="B67" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E67" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>87</v>
       </c>
       <c r="B68" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E68" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>118</v>
       </c>
       <c r="B69" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="D69" t="s">
+        <v>149</v>
+      </c>
+      <c r="E69" t="s">
+        <v>147</v>
+      </c>
+      <c r="F69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B70" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="E70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>83</v>
       </c>
       <c r="B72" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>84</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E73" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>138</v>
       </c>
@@ -1592,8 +1780,14 @@
       <c r="D75" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E75" t="s">
+        <v>147</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -1603,13 +1797,19 @@
       <c r="D76" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>153</v>
+      </c>
+      <c r="E77" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>